<commit_message>
1. Fix GN template 2. Delete unnecessary sheets in GN wb
</commit_message>
<xml_diff>
--- a/Template/GN_Template.xlsx
+++ b/Template/GN_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://biu365-my.sharepoint.com/personal/ravivav1_biu_ac_il/Documents/Documents/GitHub/bionetverification/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_E339DB8F9750F1A842F15DA5CB3521FAAB6AD127" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ECE4D32-8C7E-4421-A29B-9197D61F69B8}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_E339DB8F9750F1A842F15DA5CB3521FAAB6AD127" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{022EA954-782A-4AFD-8102-E148C4664803}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>SSP</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>General Circuit</t>
   </si>
 </sst>
 </file>
@@ -211,12 +214,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -228,17 +225,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -249,6 +246,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -568,118 +571,118 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="3"/>
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="1"/>
     </row>
     <row r="2" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="7" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="3"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L4" s="3"/>
+      <c r="L4" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -696,146 +699,146 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.5703125" style="3"/>
-    <col min="4" max="4" width="12.28515625" style="3" customWidth="1"/>
-    <col min="5" max="6" width="8.5703125" style="3"/>
-    <col min="7" max="7" width="9.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="4" customWidth="1"/>
-    <col min="15" max="1024" width="8.5703125" style="4"/>
+    <col min="1" max="3" width="8.5703125" style="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.5703125" style="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="2" customWidth="1"/>
+    <col min="15" max="1024" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:25" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
+    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Integrate Prism into General Circuit
</commit_message>
<xml_diff>
--- a/Template/GN_Template.xlsx
+++ b/Template/GN_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://biu365-my.sharepoint.com/personal/ravivav1_biu_ac_il/Documents/Documents/GitHub/bionetverification/Template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive - Bar Ilan University\Documents\GitHub\bionetverification\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_E339DB8F9750F1A842F15DA5CB3521FAAB6AD127" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{022EA954-782A-4AFD-8102-E148C4664803}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B40F3C-269B-4B2D-B5D5-0D7302ACB93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SINGLE_Template" sheetId="3" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
-  <si>
-    <t>SSP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -37,9 +34,6 @@
     <t>k</t>
   </si>
   <si>
-    <t>Set</t>
-  </si>
-  <si>
     <t>SMV No Tag File Name</t>
   </si>
   <si>
@@ -55,15 +49,9 @@
     <t>Runtime (ms)</t>
   </si>
   <si>
-    <t>Output of Interest</t>
-  </si>
-  <si>
     <t>Prism NT File Name</t>
   </si>
   <si>
-    <t>Path Exist</t>
-  </si>
-  <si>
     <t>Reachable with mu=0</t>
   </si>
   <si>
@@ -92,6 +80,12 @@
   </si>
   <si>
     <t>General Circuit</t>
+  </si>
+  <si>
+    <t>General Circuits</t>
+  </si>
+  <si>
+    <t>Depth</t>
   </si>
 </sst>
 </file>
@@ -115,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -208,11 +202,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -230,10 +237,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -248,10 +251,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -570,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -578,18 +591,18 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
       <c r="L1" s="3"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -602,30 +615,30 @@
     </row>
     <row r="2" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
+      <c r="F2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
       <c r="I2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="8"/>
       <c r="L2" s="4"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -637,28 +650,28 @@
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="2"/>
@@ -691,31 +704,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ13"/>
+  <dimension ref="A1:AMG13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.5703125" style="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="8.5703125" style="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="2" customWidth="1"/>
-    <col min="15" max="1024" width="8.5703125" style="2"/>
+    <col min="1" max="2" width="8.5703125" style="1"/>
+    <col min="3" max="3" width="12.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="2" customWidth="1"/>
+    <col min="12" max="1021" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -727,9 +739,9 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -738,53 +750,44 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="I2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="J2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="K2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -793,25 +796,22 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -820,11 +820,11 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -836,13 +836,10 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A1:N1"/>
+  <mergeCells count="12">
+    <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -854,9 +851,6 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>